<commit_message>
Updated eval and conclusion
</commit_message>
<xml_diff>
--- a/data/processed/main_experiment_results.xlsx
+++ b/data/processed/main_experiment_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Ryan\Documents\University\4th_Year\Level_4_Project\Keep-Your-Distance\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9963630A-D209-4CC0-A54D-077F325BE7FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6696C3-0308-428F-8198-C695E1CED463}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2925" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{FB0648F8-60FD-4E6A-AAF7-B25718980B1D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="4" xr2:uid="{FB0648F8-60FD-4E6A-AAF7-B25718980B1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Physical" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="98">
   <si>
     <t>Living Room</t>
   </si>
@@ -375,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -385,10 +385,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1263,16 +1264,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>2334.5900425270956</c:v>
+                    <c:v>2.3345900425270956</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>8123.6851397626187</c:v>
+                    <c:v>8.1236851397626193</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>10984.266061811626</c:v>
+                    <c:v>10.984266061811626</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7897.6791623561894</c:v>
+                    <c:v>7.8976791623561891</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1284,16 +1285,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>2334.5900425270956</c:v>
+                    <c:v>2.3345900425270956</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>8123.6851397626187</c:v>
+                    <c:v>8.1236851397626193</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>10984.266061811626</c:v>
+                    <c:v>10.984266061811626</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7897.6791623561894</c:v>
+                    <c:v>7.8976791623561891</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1336,19 +1337,19 @@
             <c:numRef>
               <c:f>'Clustered Bar Chart'!$P$2:$P$5</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1840</c:v>
+                  <c:v>1.84</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8877.75</c:v>
+                  <c:v>8.8777500000000007</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7366.75</c:v>
+                  <c:v>7.3667499999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6028.166666666667</c:v>
+                  <c:v>6.0281666666666673</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1394,16 +1395,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>5408.0114336664146</c:v>
+                    <c:v>5.4080114336664149</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2766.4480837348096</c:v>
+                    <c:v>2.7664480837348098</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2976.2498215035644</c:v>
+                    <c:v>2.9762498215035644</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3730.8574162792743</c:v>
+                    <c:v>3.7308574162792745</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1415,16 +1416,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>5408.0114336664146</c:v>
+                    <c:v>5.4080114336664149</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2766.4480837348096</c:v>
+                    <c:v>2.7664480837348098</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2976.2498215035644</c:v>
+                    <c:v>2.9762498215035644</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3730.8574162792743</c:v>
+                    <c:v>3.7308574162792745</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1467,19 +1468,19 @@
             <c:numRef>
               <c:f>'Clustered Bar Chart'!$Q$2:$Q$5</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5495.5</c:v>
+                  <c:v>5.4954999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2693.5</c:v>
+                  <c:v>2.6934999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4320.5</c:v>
+                  <c:v>4.3205</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4169.833333333333</c:v>
+                  <c:v>4.1698333333333331</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1525,16 +1526,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>5488.6479816678593</c:v>
+                    <c:v>5.4886479816678593</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2408.7247490459899</c:v>
+                    <c:v>2.40872474904599</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5746.7314405668894</c:v>
+                    <c:v>5.7467314405668892</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4708.2447285843609</c:v>
+                    <c:v>4.7082447285843605</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1546,16 +1547,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>5488.6479816678593</c:v>
+                    <c:v>5.4886479816678593</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2408.7247490459899</c:v>
+                    <c:v>2.40872474904599</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5746.7314405668894</c:v>
+                    <c:v>5.7467314405668892</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4708.2447285843609</c:v>
+                    <c:v>4.7082447285843605</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1598,19 +1599,19 @@
             <c:numRef>
               <c:f>'Clustered Bar Chart'!$R$2:$R$5</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3648</c:v>
+                  <c:v>3.6480000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2973.25</c:v>
+                  <c:v>2.9732500000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6988.75</c:v>
+                  <c:v>6.9887499999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4536.666666666667</c:v>
+                  <c:v>4.5366666666666671</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1728,7 +1729,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB" sz="1400"/>
-                  <a:t>Time taken: Lower is better (milliseconds)</a:t>
+                  <a:t>Time taken: Lower is better (seconds)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1762,7 +1763,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3360,12 +3361,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
@@ -3452,12 +3453,12 @@
       <c r="Q7" s="1"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -3530,12 +3531,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -6179,7 +6180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB863490-372B-4C46-99E7-D29050CDA671}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15:M15"/>
     </sheetView>
   </sheetViews>
@@ -8260,10 +8261,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C377AE93-C821-4BA9-9DF0-20E149062D95}">
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:AM5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P40" sqref="P40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8277,7 +8278,7 @@
     <col min="20" max="20" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -8326,8 +8327,32 @@
       <c r="W1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="AE1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -8361,36 +8386,67 @@
       <c r="O2" t="s">
         <v>0</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="9">
+        <f>AVERAGE(Results!$H$2:$H$5)/1000</f>
+        <v>1.84</v>
+      </c>
+      <c r="Q2" s="9">
+        <f>AVERAGE(Results!$H$6:$H$9)/1000</f>
+        <v>5.4954999999999998</v>
+      </c>
+      <c r="R2" s="9">
+        <f>AVERAGE(Results!$H$10:$H$13)/1000</f>
+        <v>3.6480000000000001</v>
+      </c>
+      <c r="S2" s="7"/>
+      <c r="T2" t="s">
+        <v>0</v>
+      </c>
+      <c r="U2" s="9">
+        <f>_xlfn.STDEV.S(Results!$H$2:$H$5)/1000</f>
+        <v>2.3345900425270956</v>
+      </c>
+      <c r="V2" s="9">
+        <f>_xlfn.STDEV.S(Results!$H$6:$H$9)/1000</f>
+        <v>5.4080114336664149</v>
+      </c>
+      <c r="W2" s="9">
+        <f>_xlfn.STDEV.S(Results!$H$10:$H$13)/1000</f>
+        <v>5.4886479816678593</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="2">
         <f>AVERAGE(Results!$H$2:$H$5)</f>
         <v>1840</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="AG2" s="2">
         <f>AVERAGE(Results!$H$6:$H$9)</f>
         <v>5495.5</v>
       </c>
-      <c r="R2" s="2">
+      <c r="AH2" s="2">
         <f>AVERAGE(Results!$H$10:$H$13)</f>
         <v>3648</v>
       </c>
-      <c r="S2" s="8"/>
-      <c r="T2" t="s">
+      <c r="AI2" s="7"/>
+      <c r="AJ2" t="s">
         <v>0</v>
       </c>
-      <c r="U2" s="2">
+      <c r="AK2" s="2">
         <f>_xlfn.STDEV.S(Results!$H$2:$H$5)</f>
         <v>2334.5900425270956</v>
       </c>
-      <c r="V2" s="2">
+      <c r="AL2" s="2">
         <f>_xlfn.STDEV.S(Results!$H$6:$H$9)</f>
         <v>5408.0114336664146</v>
       </c>
-      <c r="W2" s="2">
+      <c r="AM2" s="2">
         <f>_xlfn.STDEV.S(Results!$H$10:$H$13)</f>
         <v>5488.6479816678593</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>89</v>
       </c>
@@ -8424,36 +8480,67 @@
       <c r="O3" t="s">
         <v>93</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3" s="9">
+        <f>AVERAGE(Results!$H$18:$H$21)/1000</f>
+        <v>8.8777500000000007</v>
+      </c>
+      <c r="Q3" s="9">
+        <f>AVERAGE(Results!$H$22:$H$25)/1000</f>
+        <v>2.6934999999999998</v>
+      </c>
+      <c r="R3" s="9">
+        <f>AVERAGE(Results!$H$26:$H$29)/1000</f>
+        <v>2.9732500000000002</v>
+      </c>
+      <c r="S3" s="7"/>
+      <c r="T3" t="s">
+        <v>93</v>
+      </c>
+      <c r="U3" s="9">
+        <f>_xlfn.STDEV.S(Results!$H$18:$H$21)/1000</f>
+        <v>8.1236851397626193</v>
+      </c>
+      <c r="V3" s="9">
+        <f>_xlfn.STDEV.S(Results!$H$22:$H$25)/1000</f>
+        <v>2.7664480837348098</v>
+      </c>
+      <c r="W3" s="9">
+        <f>_xlfn.STDEV.S(Results!$H$26:$H$29)/1000</f>
+        <v>2.40872474904599</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF3" s="2">
         <f>AVERAGE(Results!$H$18:$H$21)</f>
         <v>8877.75</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="AG3" s="2">
         <f>AVERAGE(Results!$H$22:$H$25)</f>
         <v>2693.5</v>
       </c>
-      <c r="R3" s="2">
+      <c r="AH3" s="2">
         <f>AVERAGE(Results!$H$26:$H$29)</f>
         <v>2973.25</v>
       </c>
-      <c r="S3" s="8"/>
-      <c r="T3" t="s">
+      <c r="AI3" s="7"/>
+      <c r="AJ3" t="s">
         <v>93</v>
       </c>
-      <c r="U3" s="2">
+      <c r="AK3" s="2">
         <f>_xlfn.STDEV.S(Results!$H$18:$H$21)</f>
         <v>8123.6851397626187</v>
       </c>
-      <c r="V3" s="2">
+      <c r="AL3" s="2">
         <f>_xlfn.STDEV.S(Results!$H$22:$H$25)</f>
         <v>2766.4480837348096</v>
       </c>
-      <c r="W3" s="2">
+      <c r="AM3" s="2">
         <f>_xlfn.STDEV.S(Results!$H$26:$H$29)</f>
         <v>2408.7247490459899</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -8487,48 +8574,79 @@
       <c r="O4" t="s">
         <v>10</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="9">
+        <f>AVERAGE(Results!$H$34:$H$37)/1000</f>
+        <v>7.3667499999999997</v>
+      </c>
+      <c r="Q4" s="9">
+        <f>AVERAGE(Results!$H$38:$H$41)/1000</f>
+        <v>4.3205</v>
+      </c>
+      <c r="R4" s="9">
+        <f>AVERAGE(Results!$H$42:$H$45)/1000</f>
+        <v>6.9887499999999996</v>
+      </c>
+      <c r="S4" s="7"/>
+      <c r="T4" t="s">
+        <v>10</v>
+      </c>
+      <c r="U4" s="9">
+        <f>_xlfn.STDEV.S(Results!$H$34:$H$37)/1000</f>
+        <v>10.984266061811626</v>
+      </c>
+      <c r="V4" s="9">
+        <f>_xlfn.STDEV.S(Results!$H$38:$H$41)/1000</f>
+        <v>2.9762498215035644</v>
+      </c>
+      <c r="W4" s="9">
+        <f>_xlfn.STDEV.S(Results!$H$42:$H$45)/1000</f>
+        <v>5.7467314405668892</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF4" s="2">
         <f>AVERAGE(Results!$H$34:$H$37)</f>
         <v>7366.75</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="AG4" s="2">
         <f>AVERAGE(Results!$H$38:$H$41)</f>
         <v>4320.5</v>
       </c>
-      <c r="R4" s="2">
+      <c r="AH4" s="2">
         <f>AVERAGE(Results!$H$42:$H$45)</f>
         <v>6988.75</v>
       </c>
-      <c r="S4" s="8"/>
-      <c r="T4" t="s">
+      <c r="AI4" s="7"/>
+      <c r="AJ4" t="s">
         <v>10</v>
       </c>
-      <c r="U4" s="2">
+      <c r="AK4" s="2">
         <f>_xlfn.STDEV.S(Results!$H$34:$H$37)</f>
         <v>10984.266061811626</v>
       </c>
-      <c r="V4" s="2">
+      <c r="AL4" s="2">
         <f>_xlfn.STDEV.S(Results!$H$38:$H$41)</f>
         <v>2976.2498215035644</v>
       </c>
-      <c r="W4" s="2">
+      <c r="AM4" s="2">
         <f>_xlfn.STDEV.S(Results!$H$42:$H$45)</f>
         <v>5746.7314405668894</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <f>Results!$H$14</f>
         <v>3661.1666666666665</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <f>Results!$H$30</f>
         <v>4848.166666666667</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="7">
         <f>Results!$H$46</f>
         <v>6225.333333333333</v>
       </c>
@@ -8550,30 +8668,60 @@
       <c r="O5" t="s">
         <v>92</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="9">
+        <f>AVERAGE(Results!$H$2:$H$5,Results!$H$18:$H$21,Results!$H$34:$H$37)/1000</f>
+        <v>6.0281666666666673</v>
+      </c>
+      <c r="Q5" s="9">
+        <f>AVERAGE(Results!$H$6:$H$9,Results!$H$22:$H$25,Results!$H$38:$H$41)/1000</f>
+        <v>4.1698333333333331</v>
+      </c>
+      <c r="R5" s="9">
+        <f>AVERAGE(Results!$H$10:$H$13,Results!$H$26:$H$29,Results!$H$42:$H$45)/1000</f>
+        <v>4.5366666666666671</v>
+      </c>
+      <c r="T5" t="s">
+        <v>92</v>
+      </c>
+      <c r="U5" s="9">
+        <f>_xlfn.STDEV.S(Results!$H$2:$H$5,Results!$H$18:$H$21,Results!$H$34:$H$37)/1000</f>
+        <v>7.8976791623561891</v>
+      </c>
+      <c r="V5" s="9">
+        <f>_xlfn.STDEV.S(Results!$H$6:$H$9,Results!$H$22:$H$25,Results!$H$38:$H$41)/1000</f>
+        <v>3.7308574162792745</v>
+      </c>
+      <c r="W5" s="9">
+        <f>_xlfn.STDEV.S(Results!$H$10:$H$13,Results!$H$26:$H$29,Results!$H$42:$H$45)/1000</f>
+        <v>4.7082447285843605</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF5" s="2">
         <f>AVERAGE(Results!$H$2:$H$5,Results!$H$18:$H$21,Results!$H$34:$H$37)</f>
         <v>6028.166666666667</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="AG5" s="2">
         <f>AVERAGE(Results!$H$6:$H$9,Results!$H$22:$H$25,Results!$H$38:$H$41)</f>
         <v>4169.833333333333</v>
       </c>
-      <c r="R5" s="2">
+      <c r="AH5" s="2">
         <f>AVERAGE(Results!$H$10:$H$13,Results!$H$26:$H$29,Results!$H$42:$H$45)</f>
         <v>4536.666666666667</v>
       </c>
-      <c r="T5" t="s">
+      <c r="AJ5" t="s">
         <v>92</v>
       </c>
-      <c r="U5" s="2">
+      <c r="AK5" s="2">
         <f>_xlfn.STDEV.S(Results!$H$2:$H$5,Results!$H$18:$H$21,Results!$H$34:$H$37)</f>
         <v>7897.6791623561894</v>
       </c>
-      <c r="V5" s="2">
+      <c r="AL5" s="2">
         <f>_xlfn.STDEV.S(Results!$H$6:$H$9,Results!$H$22:$H$25,Results!$H$38:$H$41)</f>
         <v>3730.8574162792743</v>
       </c>
-      <c r="W5" s="2">
+      <c r="AM5" s="2">
         <f>_xlfn.STDEV.S(Results!$H$10:$H$13,Results!$H$26:$H$29,Results!$H$42:$H$45)</f>
         <v>4708.2447285843609</v>
       </c>

</xml_diff>